<commit_message>
feat: add most similar tokens
</commit_message>
<xml_diff>
--- a/data/raw-data/news.xlsx
+++ b/data/raw-data/news.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C522"/>
+  <dimension ref="A1:C750"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9312,6 +9312,3882 @@
         </is>
       </c>
     </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>Thủ tướng: Nâng cao chất lượng dịch vụ y tế, hướng tới mục tiêu miễn viện phí</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_608_52152342/cec85824e56a0c34557b.jpg</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thu-tuong-nang-cao-chat-luong-dich-vu-y-te-huong-toi-muc-tieu-mien-vien-phi-r52152342.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>Tổng thống Vladimir Putin: Quyết định bầu chọn người kế nhiệm thuộc về người dân Nga</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_294_52150038/6408a2211e6ff731ae7e.jpg</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tong-thong-vladimir-putin-quyet-dinh-bau-chon-nguoi-ke-nhiem-thuoc-ve-nguoi-dan-nga-r52150038.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>Biên tập viên Quang Minh và MC Vân Hugo bị phạt nặng do vi phạm về quảng cáo</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_293_52150761/aff08acd3683dfdd8692.jpg</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bien-tap-vien-quang-minh-va-mc-van-hugo-bi-phat-nang-do-vi-pham-ve-quang-cao-r52150761.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>Harry Kane vô địch cùng Bayern: Phá vỡ lời nguyền</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_23_52148949/336a5721eb6f02315b7e.jpg</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/harry-kane-vo-dich-cung-bayern-pha-vo-loi-nguyen-r52148949.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>Tâm tình những người bám công trường cao tốc Cần Thơ - Cà Mau xuyên lễ</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_04_56_52143328/d5fb81a6c2e82bb672f9.jpg</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tam-tinh-nhung-nguoi-bam-cong-truong-cao-toc-can-tho-ca-mau-xuyen-le-r52143328.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>Vụ tố 'nộp đủ tiền mới cấp cứu' ở Nam Định: Đình chỉ một số nhân viên y tế</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_608_52152118/0ee627009a4e73102a5f.jpg</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vu-to-nop-du-tien-moi-cap-cuu-o-nam-dinh-dinh-chi-mot-so-nhan-vien-y-te-r52152118.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>Cô giáo nghi bị sát hại trên đường tới trường</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_15_52149776/1863fa43460daf53f61c.jpg</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/co-giao-nghi-bi-sat-hai-tren-duong-toi-truong-r52149776.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>Sự thật thông tin tài xế bồi thường 1 tỷ cho gia đình nữ sinh tử vong ở Vĩnh Long</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_23_52151184/aafeb1160c58e506bc49.jpg</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/su-that-thong-tin-tai-xe-boi-thuong-1-ty-cho-gia-dinh-nu-sinh-tu-vong-o-vinh-long-r52151184.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>Thăm bé trai bị xe chèn qua người, Bộ trưởng Đào Hồng Lan động viên gia đình 'hãy yên tâm'</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_309_52151188/1cad1bbea7f04eae17e1.jpg</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tham-be-trai-bi-xe-chen-qua-nguoi-bo-truong-dao-hong-lan-dong-vien-gia-dinh-hay-yen-tam-r52151188.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>Ngã ngửa với ''sữa cỏ'': Quảng cáo rất bốc, chất lượng tù mù</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_608_52152116/354a19aca4e24dbc14f3.jpg</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nga-ngua-voi-sua-co-quang-cao-rat-boc-chat-luong-tu-mu-r52152116.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>Thường trực Chính phủ cho ý kiến về nhiều nội dung quan trọng</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_04_146_52144962/daf2c9ea8aa463fa3ab5.jpg</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thuong-truc-chinh-phu-cho-y-kien-ve-nhieu-noi-dung-quan-trong-r52144962.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>Cận cảnh SUV hiệu năng cao Aston Martin DBX S vừa ra mắt, mạnh 716 mã lực</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/can-canh-suv-hieu-nang-cao-aston-martin-dbx-s-vua-ra-mat-manh-716-ma-luc-r52151162.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>Giá xăng dầu giảm nhẹ</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/gia-xang-dau-giam-nhe-r52152336.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>Khai mạc trọng thể Kỳ họp thứ chín, Quốc hội khóa XV: Kỳ họp có ý nghĩa lịch sử, đưa đất nước bước vào kỷ nguyên phát triển mới</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_16_52149216/c10b505bec15054b5c04.jpg</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/khai-mac-trong-the-ky-hop-thu-chin-quoc-hoi-khoa-xv-ky-hop-co-y-nghia-lich-su-dua-dat-nuoc-buoc-vao-ky-nguyen-phat-trien-moi-r52149216.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>Tổng Bí thư: Lắng nghe ý kiến cử tri khi sửa đổi, bổ sung Hiến pháp</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tong-bi-thu-lang-nghe-y-kien-cu-tri-khi-sua-doi-bo-sung-hien-phap-r52151548.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>Đề xuất 2 nhóm nội dung trọng tâm sửa đổi, bổ sung Hiến pháp 2013</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/de-xuat-2-nhom-noi-dung-trong-tam-sua-doi-bo-sung-hien-phap-2013-r52151716.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>Ngắm 'dải lụa trắng' Phi Liêng giữa rừng già Tây Nguyên</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_04_465_52145017/9d17f706b4485d160459.jpg</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ngam-dai-lua-trang-phi-lieng-giua-rung-gia-tay-nguyen-r52145017.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>Vụ nữ sinh tử vong ở Vĩnh Long: Nhiều nhân chứng hiện trường lên tiếng</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vu-nu-sinh-tu-vong-o-vinh-long-nhieu-nhan-chung-hien-truong-len-tieng-r52149581.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>Tình trạng nghệ sĩ Thương Tín</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tinh-trang-nghe-si-thuong-tin-r52150974.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>Chưa có ai giỏi như Đoàn Văn Hậu</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chua-co-ai-gioi-nhu-doan-van-hau-r52151148.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>Xử phạt BTV Quang Minh 37,5 triệu đồng, MC Vân Hugo 70 triệu đồng</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/xu-phat-btv-quang-minh-37-5-trieu-dong-mc-van-hugo-70-trieu-dong-r52151582.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>CLIP: Tiết lộ bất ngờ của người đưa bé gái bị tai nạn giao thông ở Vĩnh Long đi cấp cứu</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/clip-tiet-lo-bat-ngo-cua-nguoi-dua-be-gai-bi-tai-nan-giao-thong-o-vinh-long-di-cap-cuu-r52151008.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>Vụ nộp đủ tiền mới cấp cứu: Bệnh viện nhận trách nhiệm, đình chỉ nhân viên có liên quan</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_114_52151337/f294fa8046ceaf90f6df.jpg</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vu-nop-du-tien-moi-cap-cuu-benh-vien-nhan-trach-nhiem-dinh-chi-nhan-vien-co-lien-quan-r52151337.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>Nổ lớn rung chuyển tòa chung cư ở Mátxcơva</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_20_52148918/d9907dd8c19628c87187.jpg</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/no-lon-rung-chuyen-toa-chung-cu-o-matxcova-r52148918.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>Tập trung điều trị, chăm sóc tốt nhất cho cháu bé bị công nông cán qua người tại Nam Định</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tap-trung-dieu-tri-cham-soc-tot-nhat-cho-chau-be-bi-cong-nong-can-qua-nguoi-tai-nam-dinh-r52151116.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>Bên trong những ngôi chùa tôn trí xá lợi Đức Phật tại Vesak 2025</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_119_52151492/b8974f83f3cd1a9343dc.jpg</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ben-trong-nhung-ngoi-chua-ton-tri-xa-loi-duc-phat-tai-vesak-2025-r52151492.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>Vụ bé trai bị từ chối cấp cứu vì chưa đóng đủ viện phí: Tạm đình chỉ một số nhân viên y tế</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vu-be-trai-bi-tu-choi-cap-cuu-vi-chua-dong-du-vien-phi-tam-dinh-chi-mot-so-nhan-vien-y-te-r52151651.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>Chiêm ngưỡng vườn đỗ quyên trong Công viên hoàng gia Richmond tại Anh</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_293_52149040/115f0f13b35d5a03034c.jpg</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chiem-nguong-vuon-do-quyen-trong-cong-vien-hoang-gia-richmond-tai-anh-r52149040.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>Chính thức vận hành chuyến tàu đặc biệt 'Hoa Phượng Đỏ' tuyến Hà Nội – Hải Phòng</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chinh-thuc-van-hanh-chuyen-tau-dac-biet-hoa-phuong-do-tuyen-ha-noi-hai-phong-r52151620.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>Tập trung phát triển kinh tế - xã hội, cải thiện đời sống của nhân dân</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tap-trung-phat-trien-kinh-te-xa-hoi-cai-thien-doi-song-cua-nhan-dan-r52150768.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>Bé sơ sinh bị ném xuống giếng: Lộ chuyện cặp đôi yêu 8 năm từng 3 lần phá thai, người mẹ khóc lóc xin sửa sai</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/be-so-sinh-bi-nem-xuong-gieng-lo-chuyen-cap-doi-yeu-8-nam-tung-3-lan-pha-thai-nguoi-me-khoc-loc-xin-sua-sai-r52150690.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>Thủ tướng Phạm Minh Chính: Đã đề xuất Bộ Chính trị, Quốc hội gỡ vướng cho hơn 2.200 dự án</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thu-tuong-pham-minh-chinh-da-de-xuat-bo-chinh-tri-quoc-hoi-go-vuong-cho-hon-2-200-du-an-r52149173.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>Tổng thống Putin: Quyết định bầu chọn người kế nhiệm thuộc về người dân Nga</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tong-thong-putin-quyet-dinh-bau-chon-nguoi-ke-nhiem-thuoc-ve-nguoi-dan-nga-r52150249.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>Chiến đấu cơ Thổ Nhĩ Kỳ xuất kích sẵn sàng bắn hạ tiêm kích Israel tấn công Syria?</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chien-dau-co-tho-nhi-ky-xuat-kich-san-sang-ban-ha-tiem-kich-israel-tan-cong-syria-r52149893.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>Kiến nghị về nâng mức xử phạt đối với hành vi điều khiển xe máy khi chưa đủ tuổi</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/kien-nghi-ve-nang-muc-xu-phat-doi-voi-hanh-vi-dieu-khien-xe-may-khi-chua-du-tuoi-r52151681.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>Xe tang cháy ngùn ngụt trên cao tốc Nội Bài - Lào Cai</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_83_52151636/5cb81aa3a6ed4fb316fc.jpg</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/xe-tang-chay-ngun-ngut-tren-cao-toc-noi-bai-lao-cai-r52151636.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>Cây xanh chết bất thường giữa TP Quảng Ngãi, nghi bị đầu độc bằng hóa chất</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w300_r3x2/2025_05_05_114_52151585/8186be9f02d1eb8fb2c0.jpg</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cay-xanh-chet-bat-thuong-giua-tp-quang-ngai-nghi-bi-dau-doc-bang-hoa-chat-r52151585.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>10 ngày tới, 4 tuổi đạt đỉnh sự nghiệp, cuối tháng giàu vỡ két</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52150997/1e503f54831a6a44330b.jpg</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/10-ngay-toi-4-tuoi-dat-dinh-su-nghiep-cuoi-thang-giau-vo-ket-r52150997.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>Tài xế ô tô tử vong khi lao vào đuôi xe tải đang lùi trên quốc lộ</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52151345/b0d8fac84686afd8f697.jpg</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tai-xe-o-to-tu-vong-khi-lao-vao-duoi-xe-tai-dang-lui-tren-quoc-lo-r52151345.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>Võ Hạ Trâm lên tiếng</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52150560/da780c4cb002595c0013.jpg</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vo-ha-tram-len-tieng-r52150560.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>Diễn biến mới vụ làm giả giấy tờ để xin cấp chứng chỉ hành nghề cho bác sĩ</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52151463/e20f201a9c54750a2c45.jpg</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dien-bien-moi-vu-lam-gia-giay-to-de-xin-cap-chung-chi-hanh-nghe-cho-bac-si-r52151463.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>Lễ thượng cờ Phật giáo tại đại lễ Vesak 2025</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52151638/99e24602fb4c12124b5d.jpg</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/le-thuong-co-phat-giao-tai-dai-le-vesak-2025-r52151638.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>Xuất hiện vết nứt kéo dài, tạm dừng lưu thông qua cầu Ka Long</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52151598/228e9f9723d9ca8793c8.jpg</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/xuat-hien-vet-nut-keo-dai-tam-dung-luu-thong-qua-cau-ka-long-r52151598.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>Giá vàng thế giới giảm mạnh, trong nước giảm nhẹ, người dân vẫn ồ ạt đi mua</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_65_52150778/1f680a54b61a5f44060b.jpg</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/gia-vang-the-gioi-giam-manh-trong-nuoc-giam-nhe-nguoi-dan-van-o-at-di-mua-r52150778.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>Dạo chơi trong công viên, người đàn ông nhặt được viên kim cương quý giá</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52151341/db21e831547fbd21e46e.jpg</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dao-choi-trong-cong-vien-nguoi-dan-ong-nhat-duoc-vien-kim-cuong-quy-gia-r52151341.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>Ông Trump nói 4 năm là đủ thời gian để làm điều gì đó 'thực sự ngoạn mục'</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_296_52151762/bc39ee25526bbb35e27a.jpg</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ong-trump-noi-4-nam-la-du-thoi-gian-de-lam-dieu-gi-do-thuc-su-ngoan-muc-r52151762.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>Sai phạm đất rừng 'treo' suốt 15 năm tại một địa phương ở Quảng Bình</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52151593/d3498b50371ede40870f.jpg</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/sai-pham-dat-rung-treo-suot-15-nam-tai-mot-dia-phuong-o-quang-binh-r52151593.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>Quy trình sửa đổi, bổ sung Hiến pháp đảm bảo chặt chẽ, cẩn trọng</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_17_52152295/34e85905e44b0d15545a.jpg</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/quy-trinh-sua-doi-bo-sung-hien-phap-dam-bao-chat-che-can-trong-r52152295.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>Vụ nộp đủ tiền mới cấp cứu bé trai bị tai nạn giao thông: Bộ trưởng Y tế Đào Hồng Lan nói gì?</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vu-nop-du-tien-moi-cap-cuu-be-trai-bi-tai-nan-giao-thong-bo-truong-y-te-dao-hong-lan-noi-gi-r52151135.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>Dự kiến lộ trình tinh giản 1.557 biên chế cấp xã của Hưng Yên</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/du-kien-lo-trinh-tinh-gian-1-557-bien-che-cap-xa-cua-hung-yen-r52151666.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>Hải Phòng hợp luyện diễu hành kỷ niệm 70 năm ngày giải phóng</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/hai-phong-hop-luyen-dieu-hanh-ky-niem-70-nam-ngay-giai-phong-r52151797.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>10 đổi mới quan trọng của Luật Khoa học Công nghệ (sửa đổi)</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52151667/c9a689b935f7dca985e6.jpg</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/10-doi-moi-quan-trong-cua-luat-khoa-hoc-cong-nghe-sua-doi-r52151667.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>TP Hồ Chí Minh: Xử phạt nhiều công ty vi phạm trong quảng cáo, kinh doanh mỹ phẩm</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52151639/4f2e1c35a07b4925106a.jpg</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tp-ho-chi-minh-xu-phat-nhieu-cong-ty-vi-pham-trong-quang-cao-kinh-doanh-my-pham-r52151639.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>Cục Người có công khẳng định không có 'liệt sĩ 6 tuổi' như thông tin trên mạng</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2_sm/2025_05_05_114_52151155/973baf31137ffa21a36e.jpg</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cuc-nguoi-co-cong-khang-dinh-khong-co-liet-si-6-tuoi-nhu-thong-tin-tren-mang-r52151155.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>Thầy giáo trẻ gục chết ngay tại văn phòng sau nhiều đêm thức trắng vì deadline</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_625_52149243/a20bf2584e16a748fe07.jpg</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thay-giao-tre-guc-chet-ngay-tai-van-phong-sau-nhieu-dem-thuc-trang-vi-deadline-r52149243.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>Người phụ nữ xin nước uống rồi tiện tay trộm cái bàn của quán cà phê</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52151487/84795b6de7230e7d5732.jpg</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nguoi-phu-nu-xin-nuoc-uong-roi-tien-tay-trom-cai-ban-cua-quan-ca-phe-r52151487.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>Đại tướng Phan Văn Giang chủ trì Hội nghị xây dựng dự án luật về lĩnh vực quân sự, quốc phòng</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_16_52151105/bbf7d4ff68b181efd8a0.jpg</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dai-tuong-phan-van-giang-chu-tri-hoi-nghi-xay-dung-du-an-luat-ve-linh-vuc-quan-su-quoc-phong-r52151105.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>Bên trong chiếc máy bay cũ Mỹ mua lại để thay thế Không lực Một của ông Trump</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/26dc73b3aef047ae1ee1.png</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ben-trong-chiec-may-bay-cu-my-mua-lai-de-thay-the-khong-luc-mot-cua-ong-trump-r52151569.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>Tổng Bí thư Tô Lâm và Phu nhân rời Hà Nội, lên đường thăm bốn nước</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52151204/2f727964c52a2c74753b.jpg</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tong-bi-thu-to-lam-va-phu-nhan-roi-ha-noi-len-duong-tham-bon-nuoc-r52151204.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>Top sự thật khó tin về loài nhện đáng sợ nhất thế giới</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52151503/af1b8c0c3042d91c8053.jpg</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/top-su-that-kho-tin-ve-loai-nhen-dang-so-nhat-the-gioi-r52151503.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>iPhone 18 sẽ có thay đổi lịch sử</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52151708/7b962b8b97c57e9b27d4.jpg</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/iphone-18-se-co-thay-doi-lich-su-r52151708.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>Lịch thi đấu và trực tiếp bán kết lượt về Cúp C1 châu Âu 2024/2025</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_65_52151360/e55da2bb1ff5f6abafe4.jpg</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/lich-thi-dau-va-truc-tiep-ban-ket-luot-ve-cup-c1-chau-au-2024-2025-r52151360.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>Cuộc chia tay âm thầm giữa người dân Mỹ và chiếc ô tô</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_309_52151668/c012a9081546fc18a557.jpg</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cuoc-chia-tay-am-tham-giua-nguoi-dan-my-va-chiec-o-to-r52151668.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>Cầu Phước Khánh trên tuyến cao tốc Bến Lức - Long Thành chính thức thi công trở lại</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cau-phuoc-khanh-tren-tuyen-cao-toc-ben-luc-long-thanh-chinh-thuc-thi-cong-tro-lai-r52151390.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>Hé lộ ảnh cận cảnh xuồng không người lái Ukraine gắn tên lửa Mỹ</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/he-lo-anh-can-canh-xuong-khong-nguoi-lai-ukraine-gan-ten-lua-my-r52151344.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>Quốc hội khóa XV: Cử tri đồng thuận cao về cuộc cách mạng tinh gọn bộ máy</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/quoc-hoi-khoa-xv-cu-tri-dong-thuan-cao-ve-cuoc-cach-mang-tinh-gon-bo-may-r52151422.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>Điều tra nguyên nhân vụ nổ khiến 1 người chết, 3 người bị thương</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dieu-tra-nguyen-nhan-vu-no-khien-1-nguoi-chet-3-nguoi-bi-thuong-r52151297.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>Đại kỳ Phật giáo lớn nhất thế giới tung bay tại Đại lễ Vesak 2025</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_65_52151517/2b238b383776de288767.jpg</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dai-ky-phat-giao-lon-nhat-the-gioi-tung-bay-tai-dai-le-vesak-2025-r52151517.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>Nhân viên sửa chữa điều hòa hoảng sợ bỏ chạy khi bình gas bất ngờ phát nổ như bom</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/16b4d28a57c7be99e7d6.png</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nhan-vien-sua-chua-dieu-hoa-hoang-so-bo-chay-khi-binh-gas-bat-ngo-phat-no-nhu-bom-r52151203.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>Cảnh báo của công an về ưu đãi 'phòng 5 sao giá 500.000 đồng/đêm'</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52151290/e60f5d01e14f0811515e.jpg</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/canh-bao-cua-cong-an-ve-uu-dai-phong-5-sao-gia-500-000-dong-dem-r52151290.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>Nghị quyết 68 của Bộ Chính trị: Phải xóa bỏ triệt để định kiến về kinh tế tư nhân Việt Nam</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150176/3364fa70463eaf60f62f.jpg</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nghi-quyet-68-cua-bo-chinh-tri-phai-xoa-bo-triet-de-dinh-kien-ve-kinh-te-tu-nhan-viet-nam-r52150176.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>Tăng trưởng GDP quý I/2025 ước đạt 6,93%</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_207_52151559/9d8126979ad973872ac8.jpg</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tang-truong-gdp-quy-i-2025-uoc-dat-6-93-r52151559.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>Nam Định chấn chỉnh tình trạng cán bộ thờ ơ, vô cảm với dân</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2_sm/2025_05_05_65_52151480/822513c5ae8b47d51e9a.jpg</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nam-dinh-chan-chinh-tinh-trang-can-bo-tho-o-vo-cam-voi-dan-r52151480.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>Đồng USD suy yếu, thị trường tài chính biến động mạnh</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_293_52151646/23df51c4ed8a04d45d9b.jpg</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dong-usd-suy-yeu-thi-truong-tai-chinh-bien-dong-manh-r52151646.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>Lịch âm 6/5 - Âm lịch hôm nay 6/5 chính xác nhất - lịch vạn niên 6/5/2025</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52151245/6627a32b1f65f63baf74.jpg</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/lich-am-6-5-am-lich-hom-nay-6-5-chinh-xac-nhat-lich-van-nien-6-5-2025-r52151245.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>2 loại rau ít 'ngậm' thuốc trừ sâu nhất chợ, nhất là cái số 1 ở quê mọc đầy</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_296_52151146/acb360b8dcf635a86ce7.jpg</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/2-loai-rau-it-ngam-thuoc-tru-sau-nhat-cho-nhat-la-cai-so-1-o-que-moc-day-r52151146.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>Bản quyền âm nhạc: Bài toán khó TikTok buộc phải giải nếu không muốn 'vỡ trận'</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52151567/6b6ea8781436fd68a427.jpg</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ban-quyen-am-nhac-bai-toan-kho-tiktok-buoc-phai-giai-neu-khong-muon-vo-tran-r52151567.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>Toàn cảnh lâu đài lớn nhất Đông Nam Á ở Ninh Bình</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52151092/597fb8760438ed66b429.jpg</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/toan-canh-lau-dai-lon-nhat-dong-nam-a-o-ninh-binh-r52151092.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>Bí ẩn ngọn núi thiêng cấm phụ nữ, đàn ông không có râu suốt hơn 1.000 năm</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52151568/8f09541fe851010f5840.jpg</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bi-an-ngon-nui-thieng-cam-phu-nu-dan-ong-khong-co-rau-suot-hon-1-000-nam-r52151568.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>Giới trẻ độc thân Trung Quốc tìm người yêu qua livestream</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52151510/00f83aef86a16fff36b0.jpg</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/gioi-tre-doc-than-trung-quoc-tim-nguoi-yeu-qua-livestream-r52151510.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>Toàn văn Nghị quyết số 68-NQ/TW của Bộ Chính trị về phát triển kinh tế tư nhân</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_65_52151019/529f668bdac5339b6ad4.jpg</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/toan-van-nghi-quyet-so-68-nq-tw-cua-bo-chinh-tri-ve-phat-trien-kinh-te-tu-nhan-r52151019.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>Lý do bất động sản thương mại tại lõi trung tâm tăng nhiệt trên toàn cầu</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_341_52151310/19234b32f77c1e22476d.jpg</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ly-do-bat-dong-san-thuong-mai-tai-loi-trung-tam-tang-nhiet-tren-toan-cau-r52151310.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>Amorim thừa nhận đáng lo ngại về Champions League</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52151104/35e858e0e4ae0df054bf.jpg</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/amorim-thua-nhan-dang-lo-ngai-ve-champions-league-r52151104.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>Đề xuất thu phí cao tốc Bến Lức - Long Thành giá 2.000 đồng/km</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/de-xuat-thu-phi-cao-toc-ben-luc-long-thanh-gia-2-000-dong-km-r52151277.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>Con gái trộm vàng, điện thoại của mẹ đưa bạn trai đem bán</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/con-gai-trom-vang-dien-thoai-cua-me-dua-ban-trai-dem-ban-r52151078.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>Hợp nhất tỉnh Bạc Liêu và Cà Mau: Phát huy tiềm năng, thế mạnh địa phương</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/hop-nhat-tinh-bac-lieu-va-ca-mau-phat-huy-tiem-nang-the-manh-dia-phuong-r52151470.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>Tại sao Đông Nam Á đặt cược lớn vào ngành công nghiệp bán dẫn?</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_3_52151703/8720d83d64738d2dd462.jpg</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tai-sao-dong-nam-a-dat-cuoc-lon-vao-nganh-cong-nghiep-ban-dan-r52151703.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>Trái Đất lộ ra hàng loạt mặt trăng mới?</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52150968/b7564f54f31a1a44430b.jpg</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/trai-dat-lo-ra-hang-loat-mat-trang-moi-r52150968.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>Vì sao một số kiến nghị của cử tri còn chậm được giải quyết?</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52151321/6314f0054c4ba515fc5a.jpg</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vi-sao-mot-so-kien-nghi-cua-cu-tri-con-cham-duoc-giai-quyet-r52151321.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>14 giờ phẫu thuật cứu thiếu nữ mắc bệnh hiếm, 10 năm chỉ ghi nhận 3 ca</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52151689/3c23dc3960778929d066.jpg</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/14-gio-phau-thuat-cuu-thieu-nu-mac-benh-hiem-10-nam-chi-ghi-nhan-3-ca-r52151689.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>Hà Nội kiểm tra nhà 'siêu mỏng, siêu méo' trên đường Nguyễn Tuân mở rộng</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52151378/a6fe57eeeba002fe5bb1.jpg</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ha-noi-kiem-tra-nha-sieu-mong-sieu-meo-tren-duong-nguyen-tuan-mo-rong-r52151378.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>Năm mục tiêu chiến lược của Mỹ đằng sau thỏa thuận khoáng sản ký với Ukraine</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2_sm/2025_05_05_294_52151442/8c3bc22e7e60973ece71.jpg</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nam-muc-tieu-chien-luoc-cua-my-dang-sau-thoa-thuan-khoang-san-ky-voi-ukraine-r52151442.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>Ca sĩ Hồng Hạnh thông báo ly hôn chồng doanh nhân hơn 18 tuổi</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52150418/4b5ef86e4420ad7ef431.jpg</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ca-si-hong-hanh-thong-bao-ly-hon-chong-doanh-nhan-hon-18-tuoi-r52150418.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>Thu ngân sách 4 tháng đầu năm 2025 tăng 26,3% so cùng kỳ năm trước</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_3_52151131/6e0f4404f84a1114485b.jpg</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thu-ngan-sach-4-thang-dau-nam-2025-tang-26-3-so-cung-ky-nam-truoc-r52151131.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>Những đối tượng sẽ bị tạm dừng chi trả lương hưu, trợ cấp bảo hiểm xã hội</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_106_52151159/57190f13b35d5a03034c.jpg</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nhung-doi-tuong-se-bi-tam-dung-chi-tra-luong-huu-tro-cap-bao-hiem-xa-hoi-r52151159.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>Ứng đủ tiền mới cấp cứu: Sự vô cảm không thể chấp nhận trong y đức</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52150764/bb1d0a0ab6445f1a0655.jpg</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ung-du-tien-moi-cap-cuu-su-vo-cam-khong-the-chap-nhan-trong-y-duc-r52150764.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>Quy mô kinh tế năm nay dự kiến vượt 500 tỷ USD, vào top 30 thế giới</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52151278/cb93a68b1ac5f39baad4.jpg</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/quy-mo-kinh-te-nam-nay-du-kien-vuot-500-ty-usd-vao-top-30-the-gioi-r52151278.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>Ái nữ Minh Nhựa bụng bầu vượt mặt vẫn cực cuốn hút</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52151313/4ec939d885966cc83587.jpg</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ai-nu-minh-nhua-bung-bau-vuot-mat-van-cuc-cuon-hut-r52151313.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>Bình Dương khai thác 'báu vật' bị lãng quên</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52151248/56e3a5ef19a1f0ffa9b0.jpg</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/binh-duong-khai-thac-bau-vat-bi-lang-quen-r52151248.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>Nguy cơ xung đột hạt nhân 'ngủ quên' giữa Ấn Độ và Pakistan trỗi dậy sau 6 năm</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_309_52151431/79417654ca1a23447a0b.jpg</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nguy-co-xung-dot-hat-nhan-ngu-quen-giua-an-do-va-pakistan-troi-day-sau-6-nam-r52151431.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>ĐH Nông Lâm TP HCM: Gói thầu sửa chữa khu nội trú tiết kiệm được 17 triệu đồng</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dh-nong-lam-tp-hcm-goi-thau-sua-chua-khu-noi-tru-tiet-kiem-duoc-17-trieu-dong-r52151371.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>Công an xác minh vụ Bệnh viện Đa khoa Nam Định bị tố 'nộp đủ tiền mới cấp cứu'</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cong-an-xac-minh-vu-benh-vien-da-khoa-nam-dinh-bi-to-nop-du-tien-moi-cap-cuu-r52150639.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>Cây bồ đề chiết từ Bồ đề thiêng sẽ được trồng tại Học viện Phật giáo Việt Nam, TP HCM</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cay-bo-de-chiet-tu-bo-de-thieng-se-duoc-trong-tai-hoc-vien-phat-giao-viet-nam-tp-hcm-r52151095.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>Tự ý dùng phương tiện cá nhân chặn đường giao thông, xử lý hành chính hay hình sự?</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52151545/17736a65d62b3f75663a.jpg</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tu-y-dung-phuong-tien-ca-nhan-chan-duong-giao-thong-xu-ly-hanh-chinh-hay-hinh-su-r52151545.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>Vụ nữ sinh tử vong ở Vĩnh Long: Hai biên bản hiện trường có 'bất thường'?</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52150123/aa0ce6265a68b336ea79.jpg</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vu-nu-sinh-tu-vong-o-vinh-long-hai-bien-ban-hien-truong-co-bat-thuong-r52150123.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>Nguyện vọng lớn nhất đời Tần Thủy Hoàng đến chết vẫn không đạt được là gì?</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52150953/c0a15da3e1ed08b351fc.jpg</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nguyen-vong-lon-nhat-doi-tan-thuy-hoang-den-chet-van-khong-dat-duoc-la-gi-r52150953.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>3 mẫu xe Ford khiến tài xế 'ôm hận' sau khi xuống tiền</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52151343/c8d681c63d88d4d68d99.jpg</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/3-mau-xe-ford-khien-tai-xe-om-han-sau-khi-xuong-tien-r52151343.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>Chi tiết CFMoto 675NK - naked bike từ Trung Quốc, chưa chốt giá bán</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52151493/9bb482a33eedd7b38efc.jpg</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chi-tiet-cfmoto-675nk-naked-bike-tu-trung-quoc-chua-chot-gia-ban-r52151493.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>Cơ quan thuế cảnh báo nguy cơ tạm hoãn xuất cảnh do nợ thuế</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52150860/6749fa484606af58f617.jpg</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/co-quan-thue-canh-bao-nguy-co-tam-hoan-xuat-canh-do-no-thue-r52150860.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>Ông Phan Văn Mãi: Lễ diễu binh, diễu hành khơi dậy khát vọng xây dựng đất nước phồn vinh</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52150314/598eb7a00beee2b0bbff.jpg</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ong-phan-van-mai-le-dieu-binh-dieu-hanh-khoi-day-khat-vong-xay-dung-dat-nuoc-phon-vinh-r52150314.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>Ngày đầu tiên vận hành hệ thống KRX: Thị trường khởi sắc nhưng còn trục trặc nhỏ</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52150917/b297c59479da9084c9cb.jpg</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ngay-dau-tien-van-hanh-he-thong-krx-thi-truong-khoi-sac-nhung-con-truc-trac-nho-r52150917.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>Bộ Công an có thư khen và thưởng 6 tập thể Công an TP.HCM</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150862/cec05cc1e08f09d1509e.jpg</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bo-cong-an-co-thu-khen-va-thuong-6-tap-the-cong-an-tp-hcm-r52150862.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>Cole Palmer phản pháo chỉ trích sau bàn thắng hạ Liverpool</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52151018/345ed25a6e14874ade05.jpg</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cole-palmer-phan-phao-chi-trich-sau-ban-thang-ha-liverpool-r52151018.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>Bảng giá ô tô Land Rover mới nhất tháng 5/2025</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52151244/dee92ae596ab7ff526ba.jpg</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bang-gia-o-to-land-rover-moi-nhat-thang-5-2025-r52151244.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>Karen Nguyễn trở lại ấn tượng trong phim kinh dị</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52151137/13ed82e63ea8d7f68eb9.jpg</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/karen-nguyen-tro-lai-an-tuong-trong-phim-kinh-di-r52151137.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>Truy tìm ẩn ý trong tranh lụa của Nguyễn Thu Hương</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52151138/7c2aee21526fbb31e27e.jpg</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/truy-tim-an-y-trong-tranh-lua-cua-nguyen-thu-huong-r52151138.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>Công Phượng đối diện nỗi buồn lớn nhất sự nghiệp</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_329_52151006/14684f6cf3221a7c4333.jpg</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cong-phuong-doi-dien-noi-buon-lon-nhat-su-nghiep-r52151006.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>Bắt giữ 2 người liên quan vụ nổ tại cảng của Iran</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bat-giu-2-nguoi-lien-quan-vu-no-tai-cang-cua-iran-r52151357.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>Cử tri bất bình về tình trạng sữa giả, thuốc giả, thực phẩm kém chất lượng</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cu-tri-bat-binh-ve-tinh-trang-sua-gia-thuoc-gia-thuc-pham-kem-chat-luong-r52150580.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>Trường đại học bỏ quy định cộng 3 điểm cho thí sinh có IELTS từ 4.0</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/truong-dai-hoc-bo-quy-dinh-cong-3-diem-cho-thi-sinh-co-ielts-tu-4-0-r52151183.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>Thủ tướng Australia và Tổng thống Mỹ Trump thảo luận về an ninh và thuế quan</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thu-tuong-australia-va-tong-thong-my-trump-thao-luan-ve-an-ninh-va-thue-quan-r52151425.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>Solskjaer phản ứng trước khó khăn của MU</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150866/4671b870043eed60b42f.jpg</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/solskjaer-phan-ung-truoc-kho-khan-cua-mu-r52150866.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>Robot hình người: Tham vọng công nghiệp mới của Trung Quốc</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_181_52151892/baa41c45a10b4855111a.jpg</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/robot-hinh-nguoi-tham-vong-cong-nghiep-moi-cua-trung-quoc-r52151892.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>Tài sản đã chia xong, con riêng có được quyền đòi hưởng thừa kế không?</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52151017/0861c2657e2b9775ce3a.jpg</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tai-san-da-chia-xong-con-rieng-co-duoc-quyen-doi-huong-thua-ke-khong-r52151017.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>Cả nước còn khoảng 60.000 biên chế được giao chưa tuyển dụng</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52151103/4c2b1e23a26d4b33127c.jpg</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ca-nuoc-con-khoang-60-000-bien-che-duoc-giao-chua-tuyen-dung-r52151103.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>Cử tri và Nhân dân bày tỏ đồng thuận, ủng hộ cao với các chủ trương lớn của Đảng và nhà nước</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_624_52150784/6a9d50a1ecef05b15cfe.jpg</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cu-tri-va-nhan-dan-bay-to-dong-thuan-ung-ho-cao-voi-cac-chu-truong-lon-cua-dang-va-nha-nuoc-r52150784.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>Tổng thống Zelensky: Ukraine có thể ngừng bắn với Nga bất cứ lúc nào</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_5_52150647/d3452e73923d7b63222c.jpg</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tong-thong-zelensky-ukraine-co-the-ngung-ban-voi-nga-bat-cu-luc-nao-r52150647.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>Đà Lạt: Hơn 160 ô tô bị phạt nguội, nhiều biển báo giao thông bị che khuất</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_17_52151432/5c5ef1494d07a459fd16.jpg</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/da-lat-hon-160-o-to-bi-phat-nguoi-nhieu-bien-bao-giao-thong-bi-che-khuat-r52151432.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>Đồng Nai: Mời thầu gói xây lắp Trạm biến áp 500kV Đồng Nai 2</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_522_52151256/9345d44a6804815ad815.jpg</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dong-nai-moi-thau-goi-xay-lap-tram-bien-ap-500kv-dong-nai-2-r52151256.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>Mạch máu càng trẻ, càng sống lâu: Bác sĩ chỉ cách kiểm tra và làm sạch mạch máu</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52151419/c0d3b4c1088fe1d1b89e.jpg</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/mach-mau-cang-tre-cang-song-lau-bac-si-chi-cach-kiem-tra-va-lam-sach-mach-mau-r52151419.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>Người đàn ông bị bắt sau 4 ngày trúng số độc đắc hơn 4.300 tỷ đồng</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52148946/c0d392982ed6c7889ec7.jpg</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nguoi-dan-ong-bi-bat-sau-4-ngay-trung-so-doc-dac-hon-4-300-ty-dong-r52148946.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>Ca tử vong nghi do bệnh dại đầu tiên trong năm 2025 tại Bà Rịa - Vũng Tàu</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52152001/94c6a7241a6af334aa7b.jpg</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ca-tu-vong-nghi-do-benh-dai-dau-tien-trong-nam-2025-tai-ba-ria-vung-tau-r52152001.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>Liên minh châu Âu tích cực 'chiêu hiền, đãi sỹ' từ Mỹ</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_293_52151141/5470fa7b4635af6bf624.jpg</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/lien-minh-chau-au-tich-cuc-chieu-hien-dai-sy-tu-my-r52151141.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>Cháy tiệm thuốc tây trên đường Vườn Lài, 2 người thoát nạn</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150760/979ab7a70be9e2b7bbf8.jpg</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chay-tiem-thuoc-tay-tren-duong-vuon-lai-2-nguoi-thoat-nan-r52150760.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>Chân dung đối tượng cướp tài sản, hiếp dâm phụ nữ đi qua đoạn đường vắng</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_106_52149477/693e0166bd2854760d39.jpg</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chan-dung-doi-tuong-cuop-tai-san-hiep-dam-phu-nu-di-qua-doan-duong-vang-r52149477.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>Mỹ lấp lỗ hổng thuế quan, Temu tuyên bố thay đổi chiến thuật</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/my-lap-lo-hong-thue-quan-temu-tuyen-bo-thay-doi-chien-thuat-r52151215.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>Đội tuyển nữ Việt Nam hội quân, hướng tới các nhiệm vụ trọng điểm năm 2025</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/doi-tuyen-nu-viet-nam-hoi-quan-huong-toi-cac-nhiem-vu-trong-diem-nam-2025-r52151291.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>Ca sĩ Tùng Dương xúc động hát Quốc ca giữa rừng cờ đỏ sao vàng tại Nhật</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ca-si-tung-duong-xuc-dong-hat-quoc-ca-giua-rung-co-do-sao-vang-tai-nhat-r52150867.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>Phát hiện voi con chết dưới giếng ở Đồng Nai... loài cực nguy cấp</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52150885/4398d89864d68d88d4c7.jpg</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/phat-hien-voi-con-chet-duoi-gieng-o-dong-nai-loai-cuc-nguy-cap-r52150885.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>Khám phá Trường thành nước ở ngoại ô thủ đô Bắc Kinh, Trung Quốc</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_14_52151581/e41fd1066d488416dd59.jpg</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/kham-pha-truong-thanh-nuoc-o-ngoai-o-thu-do-bac-kinh-trung-quoc-r52151581.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>Doanh nghiệp Mỹ điều chỉnh kế hoạch đầu tư theo chiến lược 'Nước Mỹ trước tiên'</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52150960/4196859439dad08489cb.jpg</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/doanh-nghiep-my-dieu-chinh-ke-hoach-dau-tu-theo-chien-luoc-nuoc-my-truoc-tien-r52150960.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>Có ít rau ngổ còn bổ hơn thuốc</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_94_52151629/b39997822bccc2929bdd.jpg</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/co-it-rau-ngo-con-bo-hon-thuoc-r52151629.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>Tồn trữ đồng của Trung Quốc có nguy cơ cạn kiệt vì thuế quan Mỹ</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_3_52151130/a5d3b2d80e96e7c8be87.jpg</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ton-tru-dong-cua-trung-quoc-co-nguy-co-can-kiet-vi-thue-quan-my-r52151130.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>Chốt thời gian thông xe hầm chui HC1 ở nút giao hiện đại nhất TP.HCM</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52151672/5261c77b7b35926bcb24.jpg</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chot-thoi-gian-thong-xe-ham-chui-hc1-o-nut-giao-hien-dai-nhat-tp-hcm-r52151672.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>Bình Dương: Cty Bảo Sơn Phúc, 1 ngày được chỉ định 2 gói thầu</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2_sm/2025_05_05_180_52151372/9eb465a4d9ea30b469fb.jpg</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/binh-duong-cty-bao-son-phuc-1-ngay-duoc-chi-dinh-2-goi-thau-r52151372.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>Đối thủ của MU tổn thất nặng nề</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52150316/20263417885961073848.jpg</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/doi-thu-cua-mu-ton-that-nang-ne-r52150316.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>Năm 2025, cha mẹ muốn sang tên sổ đỏ cho con nhất định phải biết những quy định này</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_625_52148023/cd7f310c8d42641c3d53.jpg</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nam-2025-cha-me-muon-sang-ten-so-do-cho-con-nhat-dinh-phai-biet-nhung-quy-dinh-nay-r52148023.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>Đại sứ Nga nêu ý nghĩa việc mời quân đội Việt Nam duyệt binh Ngày Chiến thắng</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52150455/4ae942dbfe9517cb4e84.jpg</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dai-su-nga-neu-y-nghia-viec-moi-quan-doi-viet-nam-duyet-binh-ngay-chien-thang-r52150455.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>Đường tránh Buôn Ma Thuột: Hạn chót 15/5 giải phóng mặt bằng</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52151460/3b6ef67b4a35a36bfa24.jpg</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/duong-tranh-buon-ma-thuot-han-chot-15-5-giai-phong-mat-bang-r52151460.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>Danh tính của bạn đáng giá bao nhiêu?</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_595_52151067/04c688ce3480ddde8491.jpg</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/danh-tinh-cua-ban-dang-gia-bao-nhieu-r52151067.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>'Flex' có mẹ làm công an, hot girl Bảo Khuyên khiến fan xuýt xoa</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52151093/a5384e31f27f1b21426e.jpg</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/flex-co-me-lam-cong-an-hot-girl-bao-khuyen-khien-fan-xuyt-xoa-r52151093.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>TPHCM sẵn sàng cho Đại lễ Vesak Liên Hợp Quốc lần thứ 20</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tphcm-san-sang-cho-dai-le-vesak-lien-hop-quoc-lan-thu-20-r52151332.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>Cột mốc chủ quyền - Biểu tượng thiêng liêng ở Quần đảo Trường Sa</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cot-moc-chu-quyen-bieu-tuong-thieng-lieng-o-quan-dao-truong-sa-r52151118.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>Novaland chi 1.400 tỷ mua công ty sở hữu suối nước nóng Bình Châu</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52151124/cf66906d2c23c57d9c32.jpg</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/novaland-chi-1-400-ty-mua-cong-ty-so-huu-suoi-nuoc-nong-binh-chau-r52151124.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>Khánh kiệt vì 'tìm con'</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_83_52151156/b83f8c35307bd925806a.jpg</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/khanh-kiet-vi-tim-con-r52151156.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>Đụng trúng 'kho báu' Nội Mông, cả công trường lập tức dừng hoạt động</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52150829/322e2910955e7c00254f.jpg</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dung-trung-kho-bau-noi-mong-ca-cong-truong-lap-tuc-dung-hoat-dong-r52150829.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>Tiếp tục gỡ nút thắt xử lý nợ xấu</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_95_52150891/d52c1a2ca6624f3c1673.jpg</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tiep-tuc-go-nut-that-xu-ly-no-xau-r52150891.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>Top 10 xe hạng sang bán chạy nhất tại Mỹ năm 2025</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_326_52151122/01ccfdc4418aa8d4f19b.jpg</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/top-10-xe-hang-sang-ban-chay-nhat-tai-my-nam-2025-r52151122.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>Bệnh viện Chợ Rẫy tiếp nhận gần 1.400 ca cấp cứu trong kỳ nghỉ lễ</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52151055/2e2cb42a0864e13ab875.jpg</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/benh-vien-cho-ray-tiep-nhan-gan-1-400-ca-cap-cuu-trong-ky-nghi-le-r52151055.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>Harry Kane lên tiếng sau khi Bayern Munich chính thức vô địch Bundesliga</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150769/17458f783336da688327.jpg</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/harry-kane-len-tieng-sau-khi-bayern-munich-chinh-thuc-vo-dich-bundesliga-r52150769.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>Công an vào cuộc xác minh vụ tài xế công nghệ bị hành hung</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52151168/a4b820b29cfc75a22ced.jpg</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cong-an-vao-cuoc-xac-minh-vu-tai-xe-cong-nghe-bi-hanh-hung-r52151168.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>Chuyện khó tin: Mèo rơi vào nồi lẩu khiến 9 người nhập viện ở Trung Quốc</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_15_52149259/ccca8a9836d6df8886c7.jpg</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chuyen-kho-tin-meo-roi-vao-noi-lau-khien-9-nguoi-nhap-vien-o-trung-quoc-r52149259.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>Israel tuyên bố sẽ trả đũa Houthi và Iran sau vụ tấn công sân bay</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_106_52150996/1c5d0959b5175c490506.jpg</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/israel-tuyen-bo-se-tra-dua-houthi-va-iran-sau-vu-tan-cong-san-bay-r52150996.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>Giết chồng vũ phu trong lúc bỏ trốn, người phụ nữ lĩnh án 11 năm tù</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_625_52149773/d21d033dbf73562d0f62.jpg</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/giet-chong-vu-phu-trong-luc-bo-tron-nguoi-phu-nu-linh-an-11-nam-tu-r52149773.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>Bắt đối tượng gây rối khu vực bảo vệ đoàn khách quốc tế</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/e9b048137951900fc940.png</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bat-doi-tuong-gay-roi-khu-vuc-bao-ve-doan-khach-quoc-te-r52150789.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>ASEAN+3 cảnh báo tác động từ chủ nghĩa bảo hộ</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52151089/3d44374c8b02625c3b13.jpg</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/asean-3-canh-bao-tac-dong-tu-chu-nghia-bao-ho-r52151089.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>Người đàn ông gặp nạn kinh hoàng vì cố chụp ảnh tự sướng</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_23_52150783/fa80ddbc61f288acd1e3.jpg</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nguoi-dan-ong-gap-nan-kinh-hoang-vi-co-chup-anh-tu-suong-r52150783.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>Nhặt được chìa khóa ô tô, nam thanh niên liền trộm xe, mang cất giấu</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_94_52150751/6699e5a359edb0b3e9fc.jpg</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nhat-duoc-chia-khoa-o-to-nam-thanh-nien-lien-trom-xe-mang-cat-giau-r52150751.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>Nhảy khỏi thùng xe tải, con bò bị ô tô đâm trúng</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nhay-khoi-thung-xe-tai-con-bo-bi-o-to-dam-trung-r52150923.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>Đề xuất hai phương án xử lý nền đất yếu dự án cao tốc Châu Đốc - Cần Thơ - Sóc Trăng</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/de-xuat-hai-phuong-an-xu-ly-nen-dat-yeu-du-an-cao-toc-chau-doc-can-tho-soc-trang-r52150985.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>Tổng thống Trump lên tiếng sau khi bị Tổng thống Mexico từ chối yêu cầu</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tong-thong-trump-len-tieng-sau-khi-bi-tong-thong-mexico-tu-choi-yeu-cau-r52148822.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>Hành động nhận được hàng nghìn lời khen của Đức Phúc sau đại lễ 30/4</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_181_52151296/a6f0bce100afe9f1b0be.jpg</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/hanh-dong-nhan-duoc-hang-nghin-loi-khen-cua-duc-phuc-sau-dai-le-30-4-r52151296.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>Theo quy định mới nhất, vượt xe không đúng quy định bị phạt bao nhiêu tiền?</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_296_52150922/38c2a5c1198ff0d1a99e.jpg</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/theo-quy-dinh-moi-nhat-vuot-xe-khong-dung-quy-dinh-bi-phat-bao-nhieu-tien-r52150922.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>Vietnam AutoExpo 2025 thu hút sự tham dự của hơn 180 doanh nghiệp trong nước và quốc tế</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_72_52150804/4f9d63a2dfec36b26ffd.jpg</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vietnam-autoexpo-2025-thu-hut-su-tham-du-cua-hon-180-doanh-nghiep-trong-nuoc-va-quoc-te-r52150804.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>TPHCM: Trường nào có điểm chuẩn vào lớp 10 công lập cao nhất trong 3 năm qua</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_181_52151481/be80f89444daad84f4cb.jpg</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tphcm-truong-nao-co-diem-chuan-vao-lop-10-cong-lap-cao-nhat-trong-3-nam-qua-r52151481.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>TP.HCM chi hơn 1.100 tỉ xây dựng Cung Thiếu nhi tại khu đô thị mới Thủ Thiêm</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150785/9719d0256c6b8535dc7a.jpg</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tp-hcm-chi-hon-1-100-ti-xay-dung-cung-thieu-nhi-tai-khu-do-thi-moi-thu-thiem-r52150785.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>Sáp nhập tỉnh, cán bộ tỉnh Bình Phước đi đường nào sang Đồng Nai?</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150014/1207c521796f9031c97e.jpg</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/sap-nhap-tinh-can-bo-tinh-binh-phuoc-di-duong-nao-sang-dong-nai-r52150014.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>Đèo Cả thu BOT gần 6 tỷ đồng mỗi ngày, lãi kỷ lục quý đầu năm</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52151059/998e2e8892c67b9822d7.jpg</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/deo-ca-thu-bot-gan-6-ty-dong-moi-ngay-lai-ky-luc-quy-dau-nam-r52151059.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>TP.HCM: Gấp rút tháo dỡ khán đài hơn 5.000 chỗ trên đường Lê Duẩn</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52151262/688b90842ccac5949cdb.jpg</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tp-hcm-gap-rut-thao-do-khan-dai-hon-5-000-cho-tren-duong-le-duan-r52151262.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>Kế hoạch để Venice không bị nhấn chìm</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_125_52150826/0c9de4a258ecb1b2e8fd.jpg</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ke-hoach-de-venice-khong-bi-nhan-chim-r52150826.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>Ngắm mô hình Tôn tượng Phật lớn nhất thế giới ở Thanh Hóa</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150740/9bc70dfab1b458ea01a5.jpg</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ngam-mo-hinh-ton-tuong-phat-lon-nhat-the-gioi-o-thanh-hoa-r52150740.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>Thêm nhiều nhà hàng Việt được cẩm nang ẩm thực MICHELIN vinh danh</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_65_52150744/e2586467d82931776838.jpg</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/them-nhieu-nha-hang-viet-duoc-cam-nang-am-thuc-michelin-vinh-danh-r52150744.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>Thủ tướng Thái Lan tiết lộ đang 'thảo luận bí mật' với Mỹ về thuế quan</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_595_52150946/802c5329ef6706395f76.jpg</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thu-tuong-thai-lan-tiet-lo-dang-thao-luan-bi-mat-voi-my-ve-thue-quan-r52150946.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>Giải pháp nào cho mục tiêu tăng trưởng 8%</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_59_52150964/b8ad5cafe0e109bf50f0.jpg</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/giai-phap-nao-cho-muc-tieu-tang-truong-8-r52150964.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>Kênh đào Panama 'lao đao' giữa trong cuộc chiến thương mại Mỹ - Trung</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52150951/82770375bf3b56650f2a.jpg</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/kenh-dao-panama-lao-dao-giua-trong-cuoc-chien-thuong-mai-my-trung-r52150951.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>Ông Trump nói về người kế nhiệm</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ong-trump-noi-ve-nguoi-ke-nhiem-r52150699.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>Chủ nhiệm UBKT Phan Văn Mãi: Kinh tế tư nhân chưa tạo được đột phá</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/chu-nhiem-ubkt-phan-van-mai-kinh-te-tu-nhan-chua-tao-duoc-dot-pha-r52150935.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>Dừng xe dụi mắt, hai cô gái trẻ tránh được tai nạn thảm khốc trong tích tắc</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/26dc73b3aef047ae1ee1.png</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dung-xe-dui-mat-hai-co-gai-tre-tranh-duoc-tai-nan-tham-khoc-trong-tich-tac-r52149949.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>Bộ Tư pháp ban hành Kế hoạch lấy ý kiến Nhân dân về sửa đổi, bổ sung một số điều của Hiến pháp năm 2013</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_3_52149201/8ad8da8866c68f98d6d7.jpg</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bo-tu-phap-ban-hanh-ke-hoach-lay-y-kien-nhan-dan-ve-sua-doi-bo-sung-mot-so-dieu-cua-hien-phap-nam-2013-r52149201.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>Công an phường 'khoanh vùng' nhanh nhóm người sử dụng ma túy và tàng trữ vũ khí</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_5_52151058/c07c6f7ad3343a6a6325.jpg</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cong-an-phuong-khoanh-vung-nhanh-nhom-nguoi-su-dung-ma-tuy-va-tang-tru-vu-khi-r52151058.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>Hiểu về lỗ kép trong đầu tư chứng khoán</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_95_52150399/a18b39bb85f56cab35e4.jpg</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/hieu-ve-lo-kep-trong-dau-tu-chung-khoan-r52150399.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>Nhặt viên đá lạ, tưởng miếng thịt lợn ai ngờ là 'báu vật' tiền tỷ</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52150619/b6a2f49448daa184f8cb.jpg</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nhat-vien-da-la-tuong-mieng-thit-lon-ai-ngo-la-bau-vat-tien-ty-r52150619.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>Amorim lo lắng về chấn thương nặng của trụ cột MU</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_114_52150328/628d3cbc80f269ac30e3.jpg</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/amorim-lo-lang-ve-chan-thuong-nang-cua-tru-cot-mu-r52150328.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>Nga sẵn sàng làm trung gian hòa giải Ấn Độ - Pakistan</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_14_52151303/82e6eef752b9bbe7e2a8.jpg</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nga-san-sang-lam-trung-gian-hoa-giai-an-do-pakistan-r52151303.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>Biểu dương thành tích triệt phá đường dây ma túy ở Điện Biên</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52150816/2a8bd58969c78099d9d6.jpg</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bieu-duong-thanh-tich-triet-pha-duong-day-ma-tuy-o-dien-bien-r52150816.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>Người đàn ông cởi trần, 'múa' rựa trên phố ở Bình Dương</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/e9b048137951900fc940.png</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nguoi-dan-ong-coi-tran-mua-rua-tren-pho-o-binh-duong-r52150574.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>Quảng Ngãi dừng đầu tư 3.800 tỷ đồng vào đảo Ngọc</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_180_52150920/4bbfcbbc77f29eacc7e3.jpg</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/quang-ngai-dung-dau-tu-3-800-ty-dong-vao-dao-ngoc-r52150920.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>Hà Tĩnh: Tìm thấy thi thể bé trai 12 tuổi sau hai ngày mất tích</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_56_52151649/27a58cbe30f0d9ae80e1.jpg</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ha-tinh-tim-thay-thi-the-be-trai-12-tuoi-sau-hai-ngay-mat-tich-r52151649.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>Giải cứu cá thể rùa biển quý hiếm mắc 'lưới ma' ở Quảng Ngãi</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/e9b048137951900fc940.png</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/giai-cuu-ca-the-rua-bien-quy-hiem-mac-luoi-ma-o-quang-ngai-r52150616.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>Ngày 7.5, khánh thành Cột cờ A Pa Chải</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_125_52151777/914b23579f1976472f08.jpg</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ngay-7-5-khanh-thanh-cot-co-a-pa-chai-r52151777.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>Hai ngày nữa, Việt Nam sẽ đàm phán phiên đầu tiên về thuế với Mỹ</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_112_52150322/72365007ec4905175c58.jpg</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/hai-ngay-nua-viet-nam-se-dam-phan-phien-dau-tien-ve-thue-voi-my-r52150322.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>Ứa nước mắt vì cách trả nợ 'không giống ai' của một người già bán xôi đầu ngõ</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2_sm/2025_05_05_125_52150128/eb3abe10025eeb00b24f.jpg</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/ua-nuoc-mat-vi-cach-tra-no-khong-giong-ai-cua-mot-nguoi-gia-ban-xoi-dau-ngo-r52150128.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>Bayern Munich đã đúng về Kane</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bayern-munich-da-dung-ve-kane-r52150567.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>Ngành du lịch 'đại thắng' dịp lễ 30-4 khi đón hơn 10,5 triệu lượt khách</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/nganh-du-lich-dai-thang-dip-le-30-4-khi-don-hon-10-5-trieu-luot-khach-r52150643.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>Tự đốt nhà mình 2 lần để thỏa mãn ước mơ ngắm lính cứu hỏa tác nghiệp</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tu-dot-nha-minh-2-lan-de-thoa-man-uoc-mo-ngam-linh-cuu-hoa-tac-nghiep-r52150323.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>Vì sao Tòa tuyên bác đơn kiện đòi 7,5 tỷ đồng?</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52151041/f8e500e2bcac55f20cbd.jpg</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/vi-sao-toa-tuyen-bac-don-kien-doi-7-5-ty-dong-r52151041.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>Uống nước chanh 'liều cao', người phụ nữ viêm ruột cấp phải nhập viện khẩn</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_94_52149543/8d0b4f51f31f1a41430e.jpg</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/uong-nuoc-chanh-lieu-cao-nguoi-phu-nu-viem-ruot-cap-phai-nhap-vien-khan-r52149543.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>Di tích thuyền cổ độc đáo ở Bắc Ninh có từ thời nhà Lý</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_207_52150847/fed420ea9ca475fa2cb5.jpg</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/di-tich-thuyen-co-doc-dao-o-bac-ninh-co-tu-thoi-nha-ly-r52150847.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>Thực hiện bảo vệ và phát huy giá trị di sản 'Lễ hội Vía Bà Chúa Xứ núi Sam'</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_181_52151295/31cb29da95947cca2585.jpg</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thuc-hien-bao-ve-va-phat-huy-gia-tri-di-san-le-hoi-via-ba-chua-xu-nui-sam-r52151295.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>Antony giá 100 triệu euro đã thực sự xuất hiện</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52149859/0175ec575019b947e008.jpg</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/antony-gia-100-trieu-euro-da-thuc-su-xuat-hien-r52149859.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>Bắt đối tượng trộm cắp xe máy sau 12 giờ gây án</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_236_52150893/09c6c0c67c8895d6cc99.jpg</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bat-doi-tuong-trom-cap-xe-may-sau-12-gio-gay-an-r52150893.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>Phát hiện ra nguồn gốc gây bất ngờ của vàng và các kim loại nặng trên Trái Đất</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52150552/20ada6991ad7f389aac6.jpg</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/phat-hien-ra-nguon-goc-gay-bat-ngo-cua-vang-va-cac-kim-loai-nang-tren-trai-dat-r52150552.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>Lisa gây chú ý tại giải đua xe F1</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52150851/1b0d070cbb42521c0b53.jpg</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/lisa-gay-chu-y-tai-giai-dua-xe-f1-r52150851.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>Vận hành hệ thống giao dịch mới, VN-Index tăng lên 1.231 điểm, điểm sáng cổ phiếu 'nhà' Vingroup</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_72_52150594/c5766b41d70f3e51671e.jpg</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/van-hanh-he-thong-giao-dich-moi-vn-index-tang-len-1-231-diem-diem-sang-co-phieu-nha-vingroup-r52150594.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>Cao nguyên đá Đồng Văn: Điểm sáng trong phát triển kinh tế - xã hội vùng núi phía Bắc</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_624_52150913/d9468545390bd055891a.jpg</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/cao-nguyen-da-dong-van-diem-sang-trong-phat-trien-kinh-te-xa-hoi-vung-nui-phia-bac-r52150913.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>Thủ tướng: Hoàn thiện mô hình tổ chức của hệ thống chính trị với tinh thần 'không làm nửa vời'</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_20_52150348/c9796648da0633586a17.jpg</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thu-tuong-hoan-thien-mo-hinh-to-chuc-cua-he-thong-chinh-tri-voi-tinh-than-khong-lam-nua-voi-r52150348.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>Đảng ủy Sư đoàn 390 tổng kết 10 năm thực hiện Nghị quyết 347 của Quân ủy Trung ương</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_16_52150817/87ea2bd5979b7ec5278a.jpg</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/dang-uy-su-doan-390-tong-ket-10-nam-thuc-hien-nghi-quyet-347-cua-quan-uy-trung-uong-r52150817.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>Rủi ro thuế quan đẩy ngành sản xuất Việt Nam vào đà suy giảm</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_358_52150850/9f6b996a2524cc7a9535.jpg</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/rui-ro-thue-quan-day-nganh-san-xuat-viet-nam-vao-da-suy-giam-r52150850.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>Trần Quyết Chiến vào ban chấp hành liên đoàn Billiards TP.HCM</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_119_52150747/1c346f0ed3403a1e6351.jpg</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tran-quyet-chien-vao-ban-chap-hanh-lien-doan-billiards-tp-hcm-r52150747.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>CLIP: Hoảng hồn trước màn mở cửa xe ô tô bằng răng của sư tử và cái kết gay cấn</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/clip-hoang-hon-truoc-man-mo-cua-xe-o-to-bang-rang-cua-su-tu-va-cai-ket-gay-can-r52151684.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>Sinh viên ngành Triết học có được miễn học phí?</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/sinh-vien-nganh-triet-hoc-co-duoc-mien-hoc-phi-r52150821.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>Bé 4 tuổi vụ bệnh viện bị tố 'nộp đủ tiền mới cấp cứu' không còn phải thở máy</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/be-4-tuoi-vu-benh-vien-bi-to-nop-du-tien-moi-cap-cuu-khong-con-phai-tho-may-r52149229.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>TPHCM: Hàng ngàn người đổ về chùa Thanh Tâm chiêm bái Xá lợi Phật</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAP///wAAACH5BAEAAAAALAAAAAABAAEAAAICRAEAOw==</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tphcm-hang-ngan-nguoi-do-ve-chua-thanh-tam-chiem-bai-xa-loi-phat-r52150837.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>Trung Quốc 'khát' nhân lực cổ cồn xanh lá</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_294_52150961/a85b6d59d11738496106.jpg</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/trung-quoc-khat-nhan-luc-co-con-xanh-la-r52150961.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>Bổ sung Bảo tàng Đảng Cộng sản Việt Nam vào Quy hoạch mạng lưới cơ sở văn hóa và thể thao thời kỳ 2021-2030</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_624_52150910/97c3a6c01a8ef3d0aa9f.jpg</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/bo-sung-bao-tang-dang-cong-san-viet-nam-vao-quy-hoach-mang-luoi-co-so-van-hoa-va-the-thao-thoi-ky-2021-2030-r52150910.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>Z127: Nơi luyện ý chí thép, rèn lửa Anh hùng</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_16_52150745/98a51598a9d6408819c7.jpg</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/z127-noi-luyen-y-chi-thep-ren-lua-anh-hung-r52150745.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>Tập huấn công nghệ thông tin, an toàn thông tin, an ninh mạng phục vụ chuyển đổi số năm 2025</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_16_52150818/0400a03f1c71f52fac60.jpg</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/tap-huan-cong-nghe-thong-tin-an-toan-thong-tin-an-ninh-mang-phuc-vu-chuyen-doi-so-nam-2025-r52150818.epi</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>Thành phố Hồ Chí Minh bảo đảm công tác y tế tại Đại lễ Vesak 2025</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>https://photo-baomoi.bmcdn.me/w250_r3x2/2025_05_05_14_52150952/ba4222409e0e77502e1f.jpg</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://lite.baomoi.com/thanh-pho-ho-chi-minh-bao-dam-cong-tac-y-te-tai-dai-le-vesak-2025-r52150952.epi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>